<commit_message>
i dont know what has been changed
</commit_message>
<xml_diff>
--- a/app/App-Bilder.xlsx
+++ b/app/App-Bilder.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="810" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bildersammlung" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="647">
   <si>
     <t>Autor/Psyeudonym</t>
   </si>
@@ -2140,6 +2140,24 @@
   </si>
   <si>
     <t>&lt;image&gt;&lt;resname&gt;yak&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Yak&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;yak&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;hbieser&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/yak-tier-tibet-grunzochse-642700/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;yak&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddledisliked&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddledisliked&gt;&lt;/image&gt;</t>
+  </si>
+  <si>
+    <t>Galkenmännchen mit Puzzle</t>
+  </si>
+  <si>
+    <t>100 Fragen um ein Bild aufzudecken</t>
+  </si>
+  <si>
+    <t>100 Questions</t>
+  </si>
+  <si>
+    <t>Fragen werden nach vorgefertigtem Muster gestellt (z.B. 1. Es handelt sich um ein Lebewesen; 2. Die Farbe blau ist enthalten). Systemseitig werden die Antworten als Ja/Nein erfasst und mit der Lösung überprüft (z.B. Muster Ja/Ja/Nein/Nein/Ja/…). Ist eine Antwort richtig wird die nächste Frage gestellt und eines der 100 kleinen Teile aufgedeckt. Ist die Antwort falsch, wird das Intro Männchen vom UFO aufgezogen, Rätselpower wird abgezogen oder Galgenmännchen wird gehängt</t>
+  </si>
+  <si>
+    <t>Das Bild ist verdeckt, als 100 Teile unterteilt oder durcheinander. Anstelle der einzugebenden Buchstaben befindet sich unten nur zwei Kreise mit Auswahlmöglichkeiten (z.B. Ja-Nein)</t>
+  </si>
+  <si>
+    <t>Wird eine Frage richtig gelöst, dann wird die Verdeckung weniger. Also ein Teil wird richtig sortiert, Transparenz wird verbessert oder ein Bruchstück aufgedeckt</t>
   </si>
 </sst>
 </file>
@@ -2816,7 +2834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D124" sqref="D124"/>
     </sheetView>
@@ -9989,10 +10007,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView windowProtection="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView windowProtection="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10140,6 +10158,30 @@
         <v>168</v>
       </c>
     </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
image and icon change
8 pictures added, dice icon changed (without +), app icon changed
</commit_message>
<xml_diff>
--- a/app/App-Bilder.xlsx
+++ b/app/App-Bilder.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1799" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="1269">
   <si>
     <t>Autor/Psyeudonym</t>
   </si>
@@ -3794,12 +3794,138 @@
   <si>
     <t>BE: autumn</t>
   </si>
+  <si>
+    <t>geralt</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/frage-bild-quadrat-fragezeichen-556104/</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Dice</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/statistik-kurve-verlauf-business-741629/</t>
+  </si>
+  <si>
+    <t>Statistik</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>statistik</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/filmen-projektor-filmprojektor-kino-738808/</t>
+  </si>
+  <si>
+    <t>Film</t>
+  </si>
+  <si>
+    <t>film</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/auto-scheinwerfer-licht-lampe-741504/</t>
+  </si>
+  <si>
+    <t>Scheinwerfer</t>
+  </si>
+  <si>
+    <t>spotlight</t>
+  </si>
+  <si>
+    <t>scheinwerfer</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/einkaufswagen-internet-warenkorb-728410/</t>
+  </si>
+  <si>
+    <t>Einkaufswagen</t>
+  </si>
+  <si>
+    <t>shoppingcart</t>
+  </si>
+  <si>
+    <t>einkaufswagen</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/tastatur-leer-l%C3%B6schen-gel%C3%B6scht-648438/</t>
+  </si>
+  <si>
+    <t>Tastatur</t>
+  </si>
+  <si>
+    <t>keyboard</t>
+  </si>
+  <si>
+    <t>tastatur</t>
+  </si>
+  <si>
+    <t>Alternativ http://pixabay.com/de/ampel-rot-lichtsignalanlage-628870/</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/mann-r%C3%BCcken-tattoo-schmetterling-538730/</t>
+  </si>
+  <si>
+    <t>Tattoo</t>
+  </si>
+  <si>
+    <t>tattoo</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/rahmen-bilderrahmen-umrandung-glanz-434292/</t>
+  </si>
+  <si>
+    <t>frame</t>
+  </si>
+  <si>
+    <t>rahmen</t>
+  </si>
+  <si>
+    <t>Alternativ http://pixabay.com/de/rahmen-bilderrahmen-umrandung-bunt-457344/</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/de/ring-rund-muster-bunt-kreise-449330/</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>ring</t>
+  </si>
+  <si>
+    <t>&lt;image&gt;&lt;resname&gt;statistik&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Statistik&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;statistic&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/statistik-kurve-verlauf-business-741629/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;statistik&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</t>
+  </si>
+  <si>
+    <t>&lt;image&gt;&lt;resname&gt;film&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Film&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;film&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/filmen-projektor-filmprojektor-kino-738808/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;film&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</t>
+  </si>
+  <si>
+    <t>&lt;image&gt;&lt;resname&gt;scheinwerfer&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Scheinwerfer&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;spotlight&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/auto-scheinwerfer-licht-lampe-741504/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;scheinwerfer&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</t>
+  </si>
+  <si>
+    <t>&lt;image&gt;&lt;resname&gt;einkaufswagen&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Einkaufswagen&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;shoppingcart&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/einkaufswagen-internet-warenkorb-728410/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;einkaufswagen&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</t>
+  </si>
+  <si>
+    <t>&lt;image&gt;&lt;resname&gt;tastatur&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Tastatur&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;keyboard&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/tastatur-leer-l%C3%B6schen-gel%C3%B6scht-648438/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;tastatur&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</t>
+  </si>
+  <si>
+    <t>&lt;image&gt;&lt;resname&gt;tattoo&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Tattoo&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;tattoo&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/mann-r%C3%BCcken-tattoo-schmetterling-538730/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;tattoo&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</t>
+  </si>
+  <si>
+    <t>&lt;image&gt;&lt;resname&gt;rahmen&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;rahmen&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;frame&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/rahmen-bilderrahmen-umrandung-glanz-434292/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;rahmen&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</t>
+  </si>
+  <si>
+    <t>&lt;image&gt;&lt;resname&gt;ring&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Ring&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;ring&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/ring-rund-muster-bunt-kreise-449330/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;ring&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3865,6 +3991,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -3905,7 +4037,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3943,13 +4075,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF960000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF960000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -4115,6 +4262,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF960000"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4176,19 +4326,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M222" totalsRowShown="0">
-  <autoFilter ref="A1:M222"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M230" totalsRowShown="0">
+  <autoFilter ref="A1:M230"/>
   <sortState ref="A2:M222">
     <sortCondition ref="I1:I222"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="2" name="Autor/Psyeudonym" dataDxfId="8"/>
-    <tableColumn id="3" name="ggf. Bildtitel" dataDxfId="7">
+    <tableColumn id="2" name="Autor/Psyeudonym" dataDxfId="10"/>
+    <tableColumn id="3" name="ggf. Bildtitel" dataDxfId="9">
       <calculatedColumnFormula>Tabelle1[[#This Row],[Dateiname]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Lizenzname" dataDxfId="6"/>
-    <tableColumn id="5" name="Quelle" dataDxfId="5" dataCellStyle="Link"/>
-    <tableColumn id="6" name="Modi" dataDxfId="4" dataCellStyle="Link"/>
+    <tableColumn id="4" name="Lizenzname" dataDxfId="8"/>
+    <tableColumn id="5" name="Quelle" dataDxfId="7" dataCellStyle="Link"/>
+    <tableColumn id="6" name="Modi" dataDxfId="6" dataCellStyle="Link"/>
     <tableColumn id="7" name="Auflösung"/>
     <tableColumn id="8" name="Lösung Deutsch"/>
     <tableColumn id="9" name="Englisch"/>
@@ -4212,16 +4362,16 @@
     <tableColumn id="2" name="Imagename">
       <calculatedColumnFormula>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Solution" dataDxfId="3">
+    <tableColumn id="3" name="Solution" dataDxfId="5">
       <calculatedColumnFormula>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Author" dataDxfId="2">
+    <tableColumn id="4" name="Author" dataDxfId="4">
       <calculatedColumnFormula>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Preference" dataDxfId="1">
+    <tableColumn id="5" name="Preference" dataDxfId="3">
       <calculatedColumnFormula>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Dislike" dataDxfId="0">
+    <tableColumn id="6" name="Dislike" dataDxfId="2">
       <calculatedColumnFormula>"&lt;riddledisliked&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddledisliked&gt;&lt;/image&gt;"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Summary">
@@ -4495,11 +4645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M222"/>
+  <dimension ref="A1:M230"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H231" sqref="H231"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D239" sqref="D239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4669,6 +4819,9 @@
       <c r="L5" t="s">
         <v>359</v>
       </c>
+      <c r="M5" t="s">
+        <v>1250</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -10387,21 +10540,227 @@
         <v>571</v>
       </c>
     </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A223" s="8" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B223" s="9" t="str">
+        <f>Tabelle1[[#This Row],[Dateiname]]</f>
+        <v>statistik</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D223" s="11" t="s">
+        <v>1231</v>
+      </c>
+      <c r="E223" s="16"/>
+      <c r="G223" s="21" t="s">
+        <v>1232</v>
+      </c>
+      <c r="H223" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I223" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A224" s="8" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B224" s="9" t="str">
+        <f>Tabelle1[[#This Row],[Dateiname]]</f>
+        <v>film</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D224" s="11" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E224" s="16"/>
+      <c r="G224" s="21" t="s">
+        <v>1236</v>
+      </c>
+      <c r="H224" t="s">
+        <v>1237</v>
+      </c>
+      <c r="I224" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A225" s="14" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B225" s="9" t="str">
+        <f>Tabelle1[[#This Row],[Dateiname]]</f>
+        <v>scheinwerfer</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D225" s="11" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E225" s="16"/>
+      <c r="G225" s="21" t="s">
+        <v>1239</v>
+      </c>
+      <c r="H225" t="s">
+        <v>1240</v>
+      </c>
+      <c r="I225" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A226" s="14" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B226" s="9" t="str">
+        <f>Tabelle1[[#This Row],[Dateiname]]</f>
+        <v>einkaufswagen</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D226" s="11" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E226" s="19"/>
+      <c r="G226" s="21" t="s">
+        <v>1243</v>
+      </c>
+      <c r="H226" t="s">
+        <v>1244</v>
+      </c>
+      <c r="I226" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A227" s="14" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B227" s="9" t="str">
+        <f>Tabelle1[[#This Row],[Dateiname]]</f>
+        <v>tastatur</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D227" s="11" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E227" s="19"/>
+      <c r="G227" s="21" t="s">
+        <v>1247</v>
+      </c>
+      <c r="H227" t="s">
+        <v>1248</v>
+      </c>
+      <c r="I227" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A228" s="14" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B228" s="9" t="str">
+        <f>Tabelle1[[#This Row],[Dateiname]]</f>
+        <v>tattoo</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D228" s="11" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E228" s="19"/>
+      <c r="G228" s="21" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H228" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I228" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A229" s="14" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B229" s="9" t="str">
+        <f>Tabelle1[[#This Row],[Dateiname]]</f>
+        <v>rahmen</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D229" s="11" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E229" s="19"/>
+      <c r="G229" s="21" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H229" t="s">
+        <v>1255</v>
+      </c>
+      <c r="I229" t="s">
+        <v>1256</v>
+      </c>
+      <c r="M229" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A230" s="14" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B230" s="9" t="str">
+        <f>Tabelle1[[#This Row],[Dateiname]]</f>
+        <v>ring</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D230" s="11" t="s">
+        <v>1258</v>
+      </c>
+      <c r="E230" s="19"/>
+      <c r="G230" s="21" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H230" t="s">
+        <v>1260</v>
+      </c>
+      <c r="I230" t="s">
+        <v>1260</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="ß">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="ß">
       <formula>NOT(ISERROR(SEARCH("ß",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M75 F1:F6 M7 E76:F1048576 F9:F74 E1:E74">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"NEU"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21:M22">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"NEU"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D213" r:id="rId1"/>
@@ -10609,23 +10968,31 @@
     <hyperlink ref="D93" r:id="rId203"/>
     <hyperlink ref="D102" r:id="rId204"/>
     <hyperlink ref="D207" r:id="rId205"/>
+    <hyperlink ref="D223" r:id="rId206"/>
+    <hyperlink ref="D224" r:id="rId207"/>
+    <hyperlink ref="D225" r:id="rId208"/>
+    <hyperlink ref="D226" r:id="rId209"/>
+    <hyperlink ref="D227" r:id="rId210"/>
+    <hyperlink ref="D228" r:id="rId211"/>
+    <hyperlink ref="D229" r:id="rId212"/>
+    <hyperlink ref="D230" r:id="rId213"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId206"/>
-  <drawing r:id="rId207"/>
-  <legacyDrawing r:id="rId208"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId214"/>
+  <drawing r:id="rId215"/>
+  <legacyDrawing r:id="rId216"/>
   <tableParts count="1">
-    <tablePart r:id="rId209"/>
+    <tablePart r:id="rId217"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView windowProtection="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10723,11 +11090,35 @@
         <v>905</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>558</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B2:C4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D13" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10737,7 +11128,7 @@
   <dimension ref="A1:K260"/>
   <sheetViews>
     <sheetView windowProtection="1" topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E226" sqref="E226"/>
+      <selection activeCell="M238" sqref="M238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18071,267 +18462,267 @@
       </c>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A223" t="e">
-        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B223" t="e">
-        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C223" t="e">
-        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D223" t="e">
-        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E223" t="e">
-        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F223" t="e">
-        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G223" t="e">
+      <c r="A223">
+        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
+        <v>223</v>
+      </c>
+      <c r="B223" t="str">
+        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
+        <v>&lt;image&gt;&lt;resname&gt;statistik&lt;/resname&gt;</v>
+      </c>
+      <c r="C223" t="str">
+        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
+        <v>&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Statistik&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;statistic&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;</v>
+      </c>
+      <c r="D223" t="str">
+        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
+        <v>&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/statistik-kurve-verlauf-business-741629/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;statistik&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;</v>
+      </c>
+      <c r="E223" t="str">
+        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
+        <v>&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;</v>
+      </c>
+      <c r="F223" t="str">
+        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
+        <v>&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="G223" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K223" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>&lt;image&gt;&lt;resname&gt;statistik&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Statistik&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;statistic&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/statistik-kurve-verlauf-business-741629/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;statistik&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="K223" s="3" t="s">
+        <v>1261</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A224" t="e">
-        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B224" t="e">
-        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C224" t="e">
-        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D224" t="e">
-        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E224" t="e">
-        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F224" t="e">
-        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G224" t="e">
+      <c r="A224">
+        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
+        <v>224</v>
+      </c>
+      <c r="B224" t="str">
+        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
+        <v>&lt;image&gt;&lt;resname&gt;film&lt;/resname&gt;</v>
+      </c>
+      <c r="C224" t="str">
+        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
+        <v>&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Film&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;film&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;</v>
+      </c>
+      <c r="D224" t="str">
+        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
+        <v>&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/filmen-projektor-filmprojektor-kino-738808/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;film&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;</v>
+      </c>
+      <c r="E224" t="str">
+        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
+        <v>&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;</v>
+      </c>
+      <c r="F224" t="str">
+        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
+        <v>&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="G224" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K224" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>&lt;image&gt;&lt;resname&gt;film&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Film&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;film&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/filmen-projektor-filmprojektor-kino-738808/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;film&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="K224" s="3" t="s">
+        <v>1262</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A225" t="e">
-        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B225" t="e">
-        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C225" t="e">
-        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D225" t="e">
-        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E225" t="e">
-        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F225" t="e">
-        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G225" t="e">
+      <c r="A225">
+        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
+        <v>225</v>
+      </c>
+      <c r="B225" t="str">
+        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
+        <v>&lt;image&gt;&lt;resname&gt;scheinwerfer&lt;/resname&gt;</v>
+      </c>
+      <c r="C225" t="str">
+        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
+        <v>&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Scheinwerfer&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;spotlight&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;</v>
+      </c>
+      <c r="D225" t="str">
+        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
+        <v>&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/auto-scheinwerfer-licht-lampe-741504/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;scheinwerfer&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;</v>
+      </c>
+      <c r="E225" t="str">
+        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
+        <v>&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;</v>
+      </c>
+      <c r="F225" t="str">
+        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
+        <v>&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="G225" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K225" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>&lt;image&gt;&lt;resname&gt;scheinwerfer&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Scheinwerfer&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;spotlight&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/auto-scheinwerfer-licht-lampe-741504/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;scheinwerfer&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="K225" s="3" t="s">
+        <v>1263</v>
       </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A226" t="e">
-        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B226" t="e">
-        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C226" t="e">
-        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D226" t="e">
-        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E226" t="e">
-        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F226" t="e">
-        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G226" t="e">
+      <c r="A226">
+        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
+        <v>226</v>
+      </c>
+      <c r="B226" t="str">
+        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
+        <v>&lt;image&gt;&lt;resname&gt;einkaufswagen&lt;/resname&gt;</v>
+      </c>
+      <c r="C226" t="str">
+        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
+        <v>&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Einkaufswagen&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;shoppingcart&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;</v>
+      </c>
+      <c r="D226" t="str">
+        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
+        <v>&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/einkaufswagen-internet-warenkorb-728410/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;einkaufswagen&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;</v>
+      </c>
+      <c r="E226" t="str">
+        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
+        <v>&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;</v>
+      </c>
+      <c r="F226" t="str">
+        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
+        <v>&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="G226" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K226" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>&lt;image&gt;&lt;resname&gt;einkaufswagen&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Einkaufswagen&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;shoppingcart&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/einkaufswagen-internet-warenkorb-728410/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;einkaufswagen&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="K226" s="3" t="s">
+        <v>1264</v>
       </c>
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A227" t="e">
-        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B227" t="e">
-        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C227" t="e">
-        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D227" t="e">
-        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E227" t="e">
-        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F227" t="e">
-        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G227" t="e">
+      <c r="A227">
+        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
+        <v>227</v>
+      </c>
+      <c r="B227" t="str">
+        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
+        <v>&lt;image&gt;&lt;resname&gt;tastatur&lt;/resname&gt;</v>
+      </c>
+      <c r="C227" t="str">
+        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
+        <v>&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Tastatur&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;keyboard&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;</v>
+      </c>
+      <c r="D227" t="str">
+        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
+        <v>&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/tastatur-leer-l%C3%B6schen-gel%C3%B6scht-648438/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;tastatur&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;</v>
+      </c>
+      <c r="E227" t="str">
+        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
+        <v>&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;</v>
+      </c>
+      <c r="F227" t="str">
+        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
+        <v>&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="G227" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K227" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>&lt;image&gt;&lt;resname&gt;tastatur&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Tastatur&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;keyboard&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/tastatur-leer-l%C3%B6schen-gel%C3%B6scht-648438/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;tastatur&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="K227" s="3" t="s">
+        <v>1265</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A228" t="e">
-        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B228" t="e">
-        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C228" t="e">
-        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D228" t="e">
-        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E228" t="e">
-        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F228" t="e">
-        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G228" t="e">
+      <c r="A228">
+        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
+        <v>228</v>
+      </c>
+      <c r="B228" t="str">
+        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
+        <v>&lt;image&gt;&lt;resname&gt;tattoo&lt;/resname&gt;</v>
+      </c>
+      <c r="C228" t="str">
+        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
+        <v>&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Tattoo&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;tattoo&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;</v>
+      </c>
+      <c r="D228" t="str">
+        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
+        <v>&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/mann-r%C3%BCcken-tattoo-schmetterling-538730/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;tattoo&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;</v>
+      </c>
+      <c r="E228" t="str">
+        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
+        <v>&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;</v>
+      </c>
+      <c r="F228" t="str">
+        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
+        <v>&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="G228" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K228" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>&lt;image&gt;&lt;resname&gt;tattoo&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Tattoo&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;tattoo&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/mann-r%C3%BCcken-tattoo-schmetterling-538730/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;tattoo&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="K228" s="3" t="s">
+        <v>1266</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A229" t="e">
-        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B229" t="e">
-        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C229" t="e">
-        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D229" t="e">
-        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E229" t="e">
-        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F229" t="e">
-        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G229" t="e">
+      <c r="A229">
+        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
+        <v>229</v>
+      </c>
+      <c r="B229" t="str">
+        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
+        <v>&lt;image&gt;&lt;resname&gt;rahmen&lt;/resname&gt;</v>
+      </c>
+      <c r="C229" t="str">
+        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
+        <v>&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;rahmen&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;frame&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;</v>
+      </c>
+      <c r="D229" t="str">
+        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
+        <v>&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/rahmen-bilderrahmen-umrandung-glanz-434292/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;rahmen&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;</v>
+      </c>
+      <c r="E229" t="str">
+        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
+        <v>&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;</v>
+      </c>
+      <c r="F229" t="str">
+        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
+        <v>&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="G229" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K229" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>&lt;image&gt;&lt;resname&gt;rahmen&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;rahmen&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;frame&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/rahmen-bilderrahmen-umrandung-glanz-434292/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;rahmen&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="K229" s="3" t="s">
+        <v>1267</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A230" t="e">
-        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B230" t="e">
-        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C230" t="e">
-        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D230" t="e">
-        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E230" t="e">
-        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F230" t="e">
-        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G230" t="e">
+      <c r="A230">
+        <f>ROW(Tabelle1[[#This Row],[Autor/Psyeudonym]])</f>
+        <v>230</v>
+      </c>
+      <c r="B230" t="str">
+        <f>"&lt;image&gt;&lt;resname&gt;"&amp;Tabelle1[[#This Row],[Dateiname]]&amp;"&lt;/resname&gt;"</f>
+        <v>&lt;image&gt;&lt;resname&gt;ring&lt;/resname&gt;</v>
+      </c>
+      <c r="C230" t="str">
+        <f>"&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Lösung Deutsch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;"&amp;Tabelle1[[#This Row],[Englisch]]&amp;"&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;"</f>
+        <v>&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Ring&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;ring&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;</v>
+      </c>
+      <c r="D230" t="str">
+        <f>"&lt;author&gt;&lt;name&gt;"&amp;Tabelle1[[#This Row],[Autor/Psyeudonym]]&amp;"&lt;/name&gt;&lt;source&gt;"&amp;Tabelle1[[#This Row],[Quelle]]&amp;"&lt;/source&gt;&lt;license&gt;"&amp;Tabelle1[[#This Row],[Lizenzname]]&amp;"&lt;/license&gt;&lt;title&gt;"&amp;Tabelle1[[#This Row],[ggf. Bildtitel]]&amp;"&lt;/title&gt;&lt;extras&gt;"&amp;Tabelle1[[#This Row],[Modi]]&amp;"&lt;/extras&gt;&lt;/author&gt;"</f>
+        <v>&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/ring-rund-muster-bunt-kreise-449330/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;ring&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;</v>
+      </c>
+      <c r="E230" t="str">
+        <f>"&lt;riddleprefs&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Preference]]&amp;"&lt;/type&gt;&lt;/riddleprefs&gt;"</f>
+        <v>&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;</v>
+      </c>
+      <c r="F230" t="str">
+        <f>"&lt;riddlerefused&gt;&lt;type&gt;"&amp;Tabelle1[[#This Row],[Refused]]&amp;"&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;"</f>
+        <v>&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="G230" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K230" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>&lt;image&gt;&lt;resname&gt;ring&lt;/resname&gt;&lt;solutions&gt;&lt;solution&gt;&lt;tongue&gt;de&lt;/tongue&gt;&lt;word&gt;Ring&lt;/word&gt;&lt;/solution&gt;&lt;solution&gt;&lt;tongue&gt;en&lt;/tongue&gt;&lt;word&gt;ring&lt;/word&gt;&lt;/solution&gt;&lt;/solutions&gt;&lt;author&gt;&lt;name&gt;geralt&lt;/name&gt;&lt;source&gt;http://pixabay.com/de/ring-rund-muster-bunt-kreise-449330/&lt;/source&gt;&lt;license&gt;CC0 Public Domain&lt;/license&gt;&lt;title&gt;ring&lt;/title&gt;&lt;extras&gt;&lt;/extras&gt;&lt;/author&gt;&lt;riddleprefs&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddleprefs&gt;&lt;riddlerefused&gt;&lt;type&gt;&lt;/type&gt;&lt;/riddlerefused&gt;&lt;/image&gt;</v>
+      </c>
+      <c r="K230" s="3" t="s">
+        <v>1268</v>
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>